<commit_message>
1. change deal model  and delete comment
</commit_message>
<xml_diff>
--- a/hasoffer.admin/src/main/webapp/download/Deal表格模板.xlsx
+++ b/hasoffer.admin/src/main/webapp/download/Deal表格模板.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>网站名</t>
   </si>
@@ -73,6 +73,10 @@
   </si>
   <si>
     <t>Deal描述</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2016/10/30</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -80,7 +84,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +127,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -147,11 +159,10 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -165,6 +176,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -462,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -478,22 +491,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="81">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>16</v>
       </c>
     </row>
@@ -507,8 +520,8 @@
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3">
-        <v>42412</v>
+      <c r="D2" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -521,35 +534,303 @@
       <c r="B3">
         <v>555555</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3">
-        <v>42443</v>
+      <c r="D3" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3">
-        <v>42443</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="D4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
     </row>
+    <row r="5" spans="1:6">
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="D11" s="10"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="D13" s="10"/>
+    </row>
     <row r="14" spans="1:6" ht="15">
-      <c r="E14" s="6"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="D15" s="10"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="D16" s="10"/>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="D17" s="10"/>
+    </row>
+    <row r="18" spans="4:4">
+      <c r="D18" s="10"/>
+    </row>
+    <row r="19" spans="4:4">
+      <c r="D19" s="10"/>
+    </row>
+    <row r="20" spans="4:4">
+      <c r="D20" s="10"/>
+    </row>
+    <row r="21" spans="4:4">
+      <c r="D21" s="10"/>
+    </row>
+    <row r="22" spans="4:4">
+      <c r="D22" s="10"/>
+    </row>
+    <row r="23" spans="4:4">
+      <c r="D23" s="10"/>
+    </row>
+    <row r="24" spans="4:4">
+      <c r="D24" s="10"/>
+    </row>
+    <row r="25" spans="4:4">
+      <c r="D25" s="10"/>
+    </row>
+    <row r="26" spans="4:4">
+      <c r="D26" s="10"/>
+    </row>
+    <row r="27" spans="4:4">
+      <c r="D27" s="10"/>
+    </row>
+    <row r="28" spans="4:4">
+      <c r="D28" s="10"/>
+    </row>
+    <row r="29" spans="4:4">
+      <c r="D29" s="10"/>
+    </row>
+    <row r="30" spans="4:4">
+      <c r="D30" s="10"/>
+    </row>
+    <row r="31" spans="4:4">
+      <c r="D31" s="10"/>
+    </row>
+    <row r="32" spans="4:4">
+      <c r="D32" s="10"/>
+    </row>
+    <row r="33" spans="4:4">
+      <c r="D33" s="10"/>
+    </row>
+    <row r="34" spans="4:4">
+      <c r="D34" s="10"/>
+    </row>
+    <row r="35" spans="4:4">
+      <c r="D35" s="10"/>
+    </row>
+    <row r="36" spans="4:4">
+      <c r="D36" s="10"/>
+    </row>
+    <row r="37" spans="4:4">
+      <c r="D37" s="10"/>
+    </row>
+    <row r="38" spans="4:4">
+      <c r="D38" s="10"/>
+    </row>
+    <row r="39" spans="4:4">
+      <c r="D39" s="10"/>
+    </row>
+    <row r="40" spans="4:4">
+      <c r="D40" s="10"/>
+    </row>
+    <row r="41" spans="4:4">
+      <c r="D41" s="10"/>
+    </row>
+    <row r="42" spans="4:4">
+      <c r="D42" s="10"/>
+    </row>
+    <row r="43" spans="4:4">
+      <c r="D43" s="10"/>
+    </row>
+    <row r="44" spans="4:4">
+      <c r="D44" s="10"/>
+    </row>
+    <row r="45" spans="4:4">
+      <c r="D45" s="10"/>
+    </row>
+    <row r="46" spans="4:4">
+      <c r="D46" s="10"/>
+    </row>
+    <row r="47" spans="4:4">
+      <c r="D47" s="10"/>
+    </row>
+    <row r="48" spans="4:4">
+      <c r="D48" s="10"/>
+    </row>
+    <row r="49" spans="4:4">
+      <c r="D49" s="10"/>
+    </row>
+    <row r="50" spans="4:4">
+      <c r="D50" s="10"/>
+    </row>
+    <row r="51" spans="4:4">
+      <c r="D51" s="10"/>
+    </row>
+    <row r="52" spans="4:4">
+      <c r="D52" s="10"/>
+    </row>
+    <row r="53" spans="4:4">
+      <c r="D53" s="10"/>
+    </row>
+    <row r="54" spans="4:4">
+      <c r="D54" s="10"/>
+    </row>
+    <row r="55" spans="4:4">
+      <c r="D55" s="10"/>
+    </row>
+    <row r="56" spans="4:4">
+      <c r="D56" s="10"/>
+    </row>
+    <row r="57" spans="4:4">
+      <c r="D57" s="10"/>
+    </row>
+    <row r="58" spans="4:4">
+      <c r="D58" s="10"/>
+    </row>
+    <row r="59" spans="4:4">
+      <c r="D59" s="10"/>
+    </row>
+    <row r="60" spans="4:4">
+      <c r="D60" s="10"/>
+    </row>
+    <row r="61" spans="4:4">
+      <c r="D61" s="10"/>
+    </row>
+    <row r="62" spans="4:4">
+      <c r="D62" s="10"/>
+    </row>
+    <row r="63" spans="4:4">
+      <c r="D63" s="10"/>
+    </row>
+    <row r="64" spans="4:4">
+      <c r="D64" s="10"/>
+    </row>
+    <row r="65" spans="4:4">
+      <c r="D65" s="10"/>
+    </row>
+    <row r="66" spans="4:4">
+      <c r="D66" s="10"/>
+    </row>
+    <row r="67" spans="4:4">
+      <c r="D67" s="10"/>
+    </row>
+    <row r="68" spans="4:4">
+      <c r="D68" s="10"/>
+    </row>
+    <row r="69" spans="4:4">
+      <c r="D69" s="10"/>
+    </row>
+    <row r="70" spans="4:4">
+      <c r="D70" s="10"/>
+    </row>
+    <row r="71" spans="4:4">
+      <c r="D71" s="10"/>
+    </row>
+    <row r="72" spans="4:4">
+      <c r="D72" s="10"/>
+    </row>
+    <row r="73" spans="4:4">
+      <c r="D73" s="10"/>
+    </row>
+    <row r="74" spans="4:4">
+      <c r="D74" s="10"/>
+    </row>
+    <row r="75" spans="4:4">
+      <c r="D75" s="10"/>
+    </row>
+    <row r="76" spans="4:4">
+      <c r="D76" s="10"/>
+    </row>
+    <row r="77" spans="4:4">
+      <c r="D77" s="10"/>
+    </row>
+    <row r="78" spans="4:4">
+      <c r="D78" s="10"/>
+    </row>
+    <row r="79" spans="4:4">
+      <c r="D79" s="10"/>
+    </row>
+    <row r="80" spans="4:4">
+      <c r="D80" s="10"/>
+    </row>
+    <row r="81" spans="4:4">
+      <c r="D81" s="10"/>
+    </row>
+    <row r="82" spans="4:4">
+      <c r="D82" s="10"/>
+    </row>
+    <row r="83" spans="4:4">
+      <c r="D83" s="10"/>
+    </row>
+    <row r="84" spans="4:4">
+      <c r="D84" s="10"/>
+    </row>
+    <row r="85" spans="4:4">
+      <c r="D85" s="10"/>
+    </row>
+    <row r="86" spans="4:4">
+      <c r="D86" s="10"/>
+    </row>
+    <row r="87" spans="4:4">
+      <c r="D87" s="10"/>
+    </row>
+    <row r="88" spans="4:4">
+      <c r="D88" s="10"/>
+    </row>
+    <row r="89" spans="4:4">
+      <c r="D89" s="10"/>
+    </row>
+    <row r="90" spans="4:4">
+      <c r="D90" s="10"/>
+    </row>
+    <row r="91" spans="4:4">
+      <c r="D91" s="10"/>
+    </row>
+    <row r="92" spans="4:4">
+      <c r="D92" s="10"/>
+    </row>
+    <row r="93" spans="4:4">
+      <c r="D93" s="10"/>
+    </row>
+    <row r="94" spans="4:4">
+      <c r="D94" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -559,5 +840,6 @@
     <hyperlink ref="C4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1. change deal model
</commit_message>
<xml_diff>
--- a/hasoffer.admin/src/main/webapp/download/Deal表格模板.xlsx
+++ b/hasoffer.admin/src/main/webapp/download/Deal表格模板.xlsx
@@ -47,44 +47,44 @@
   </si>
   <si>
     <t>http://www.baidu.com</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Deal价格描述</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>5 CashBack</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>50% off</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>3799</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Deal失效日期
 （格式为：2016/6/20 可为空 
 若为空则默认失效日期为当前日期的7天后）</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Deal描述</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>2016/10/30</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,12 +114,6 @@
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -159,13 +153,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -176,8 +169,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -475,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F94"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -491,22 +484,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="81">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>16</v>
       </c>
     </row>
@@ -520,7 +513,7 @@
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E2" t="s">
@@ -537,7 +530,7 @@
       <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E3" t="s">
@@ -554,286 +547,18 @@
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="D5" s="10"/>
     </row>
-    <row r="6" spans="1:6">
-      <c r="D6" s="10"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="D7" s="10"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="D8" s="10"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="D9" s="10"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="D10" s="10"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="D11" s="10"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="D12" s="10"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="D13" s="10"/>
-    </row>
-    <row r="14" spans="1:6" ht="15">
-      <c r="D14" s="10"/>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="D15" s="10"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="D16" s="10"/>
-    </row>
-    <row r="17" spans="4:4">
-      <c r="D17" s="10"/>
-    </row>
-    <row r="18" spans="4:4">
-      <c r="D18" s="10"/>
-    </row>
-    <row r="19" spans="4:4">
-      <c r="D19" s="10"/>
-    </row>
-    <row r="20" spans="4:4">
-      <c r="D20" s="10"/>
-    </row>
-    <row r="21" spans="4:4">
-      <c r="D21" s="10"/>
-    </row>
-    <row r="22" spans="4:4">
-      <c r="D22" s="10"/>
-    </row>
-    <row r="23" spans="4:4">
-      <c r="D23" s="10"/>
-    </row>
-    <row r="24" spans="4:4">
-      <c r="D24" s="10"/>
-    </row>
-    <row r="25" spans="4:4">
-      <c r="D25" s="10"/>
-    </row>
-    <row r="26" spans="4:4">
-      <c r="D26" s="10"/>
-    </row>
-    <row r="27" spans="4:4">
-      <c r="D27" s="10"/>
-    </row>
-    <row r="28" spans="4:4">
-      <c r="D28" s="10"/>
-    </row>
-    <row r="29" spans="4:4">
-      <c r="D29" s="10"/>
-    </row>
-    <row r="30" spans="4:4">
-      <c r="D30" s="10"/>
-    </row>
-    <row r="31" spans="4:4">
-      <c r="D31" s="10"/>
-    </row>
-    <row r="32" spans="4:4">
-      <c r="D32" s="10"/>
-    </row>
-    <row r="33" spans="4:4">
-      <c r="D33" s="10"/>
-    </row>
-    <row r="34" spans="4:4">
-      <c r="D34" s="10"/>
-    </row>
-    <row r="35" spans="4:4">
-      <c r="D35" s="10"/>
-    </row>
-    <row r="36" spans="4:4">
-      <c r="D36" s="10"/>
-    </row>
-    <row r="37" spans="4:4">
-      <c r="D37" s="10"/>
-    </row>
-    <row r="38" spans="4:4">
-      <c r="D38" s="10"/>
-    </row>
-    <row r="39" spans="4:4">
-      <c r="D39" s="10"/>
-    </row>
-    <row r="40" spans="4:4">
-      <c r="D40" s="10"/>
-    </row>
-    <row r="41" spans="4:4">
-      <c r="D41" s="10"/>
-    </row>
-    <row r="42" spans="4:4">
-      <c r="D42" s="10"/>
-    </row>
-    <row r="43" spans="4:4">
-      <c r="D43" s="10"/>
-    </row>
-    <row r="44" spans="4:4">
-      <c r="D44" s="10"/>
-    </row>
-    <row r="45" spans="4:4">
-      <c r="D45" s="10"/>
-    </row>
-    <row r="46" spans="4:4">
-      <c r="D46" s="10"/>
-    </row>
-    <row r="47" spans="4:4">
-      <c r="D47" s="10"/>
-    </row>
-    <row r="48" spans="4:4">
-      <c r="D48" s="10"/>
-    </row>
-    <row r="49" spans="4:4">
-      <c r="D49" s="10"/>
-    </row>
-    <row r="50" spans="4:4">
-      <c r="D50" s="10"/>
-    </row>
-    <row r="51" spans="4:4">
-      <c r="D51" s="10"/>
-    </row>
-    <row r="52" spans="4:4">
-      <c r="D52" s="10"/>
-    </row>
-    <row r="53" spans="4:4">
-      <c r="D53" s="10"/>
-    </row>
-    <row r="54" spans="4:4">
-      <c r="D54" s="10"/>
-    </row>
-    <row r="55" spans="4:4">
-      <c r="D55" s="10"/>
-    </row>
-    <row r="56" spans="4:4">
-      <c r="D56" s="10"/>
-    </row>
-    <row r="57" spans="4:4">
-      <c r="D57" s="10"/>
-    </row>
-    <row r="58" spans="4:4">
-      <c r="D58" s="10"/>
-    </row>
-    <row r="59" spans="4:4">
-      <c r="D59" s="10"/>
-    </row>
-    <row r="60" spans="4:4">
-      <c r="D60" s="10"/>
-    </row>
-    <row r="61" spans="4:4">
-      <c r="D61" s="10"/>
-    </row>
-    <row r="62" spans="4:4">
-      <c r="D62" s="10"/>
-    </row>
-    <row r="63" spans="4:4">
-      <c r="D63" s="10"/>
-    </row>
-    <row r="64" spans="4:4">
-      <c r="D64" s="10"/>
-    </row>
-    <row r="65" spans="4:4">
-      <c r="D65" s="10"/>
-    </row>
-    <row r="66" spans="4:4">
-      <c r="D66" s="10"/>
-    </row>
-    <row r="67" spans="4:4">
-      <c r="D67" s="10"/>
-    </row>
-    <row r="68" spans="4:4">
-      <c r="D68" s="10"/>
-    </row>
-    <row r="69" spans="4:4">
-      <c r="D69" s="10"/>
-    </row>
-    <row r="70" spans="4:4">
-      <c r="D70" s="10"/>
-    </row>
-    <row r="71" spans="4:4">
-      <c r="D71" s="10"/>
-    </row>
-    <row r="72" spans="4:4">
-      <c r="D72" s="10"/>
-    </row>
-    <row r="73" spans="4:4">
-      <c r="D73" s="10"/>
-    </row>
-    <row r="74" spans="4:4">
-      <c r="D74" s="10"/>
-    </row>
-    <row r="75" spans="4:4">
-      <c r="D75" s="10"/>
-    </row>
-    <row r="76" spans="4:4">
-      <c r="D76" s="10"/>
-    </row>
-    <row r="77" spans="4:4">
-      <c r="D77" s="10"/>
-    </row>
-    <row r="78" spans="4:4">
-      <c r="D78" s="10"/>
-    </row>
-    <row r="79" spans="4:4">
-      <c r="D79" s="10"/>
-    </row>
-    <row r="80" spans="4:4">
-      <c r="D80" s="10"/>
-    </row>
-    <row r="81" spans="4:4">
-      <c r="D81" s="10"/>
-    </row>
-    <row r="82" spans="4:4">
-      <c r="D82" s="10"/>
-    </row>
-    <row r="83" spans="4:4">
-      <c r="D83" s="10"/>
-    </row>
-    <row r="84" spans="4:4">
-      <c r="D84" s="10"/>
-    </row>
-    <row r="85" spans="4:4">
-      <c r="D85" s="10"/>
-    </row>
-    <row r="86" spans="4:4">
-      <c r="D86" s="10"/>
-    </row>
-    <row r="87" spans="4:4">
-      <c r="D87" s="10"/>
-    </row>
-    <row r="88" spans="4:4">
-      <c r="D88" s="10"/>
-    </row>
-    <row r="89" spans="4:4">
-      <c r="D89" s="10"/>
-    </row>
-    <row r="90" spans="4:4">
-      <c r="D90" s="10"/>
-    </row>
-    <row r="91" spans="4:4">
-      <c r="D91" s="10"/>
-    </row>
-    <row r="92" spans="4:4">
-      <c r="D92" s="10"/>
-    </row>
-    <row r="93" spans="4:4">
-      <c r="D93" s="10"/>
-    </row>
-    <row r="94" spans="4:4">
-      <c r="D94" s="10"/>
-    </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" tooltip="http://www.baidu.com"/>
     <hyperlink ref="C3" r:id="rId2"/>

</xml_diff>